<commit_message>
get data in relation table
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sadique\Flask\File_parser\Excel to DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95033ACE-AD66-4B3E-B5DA-18D4095D1E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20DFEE9-B813-43F6-B010-ADFD6618DC27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3870" activeTab="2" xr2:uid="{D9A66578-B192-43D7-866F-924323FDCE10}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3870" xr2:uid="{D9A66578-B192-43D7-866F-924323FDCE10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FCD3AD-F989-4C12-91CB-7B8914570498}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FC0358-66E8-4473-B31B-12B98B9AB630}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>